<commit_message>
Fixed some aspects of the error analysis
</commit_message>
<xml_diff>
--- a/validation_study_files/validation_study_pitch.xlsx
+++ b/validation_study_files/validation_study_pitch.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jafri\Documents\GitHub\RAO-Research\validation_study_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EEBD7AB-6EBD-40F5-B988-697227BA4369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD351FF6-F54E-4192-BA3B-5527E5B34854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{12409B75-DDE9-4E79-996F-CF0147769801}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{12409B75-DDE9-4E79-996F-CF0147769801}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -359,7 +359,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Seung et al (Strip Theory)</c:v>
+            <c:v>Lee et al (Strip Theory)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -522,7 +522,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Me (ANSYS)</c:v>
+            <c:v>Present Study (ANSYS)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -1911,7 +1911,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Edited Paper, added todos in code
</commit_message>
<xml_diff>
--- a/validation_study_files/validation_study_pitch.xlsx
+++ b/validation_study_files/validation_study_pitch.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jafri\Documents\GitHub\RAO-Research\validation_study_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1CC5CC-4937-4BAC-AA12-CEA9CA651865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC686B6B-4C96-4B46-B6EB-6F1CCACD1C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{12409B75-DDE9-4E79-996F-CF0147769801}"/>
+    <workbookView xWindow="7290" yWindow="4905" windowWidth="21600" windowHeight="11295" xr2:uid="{12409B75-DDE9-4E79-996F-CF0147769801}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -211,161 +211,10 @@
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Patel (ANSYS)</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$3:$A$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
-                <c:pt idx="0">
-                  <c:v>0.30064478064815198</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.36392178347170101</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.41569387669096902</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.46746596991023598</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.51923806312950405</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.57101015634877195</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.62853470437018</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.72057398120443295</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.80686080323654596</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.84712798685153201</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.87397277592818901</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.89314762526865898</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.91999241434531598</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.93916726368578496</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.97368199249862997</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.00819672131147</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.0714737241350201</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.1922752749799801</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$3:$B$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
-                <c:pt idx="0">
-                  <c:v>7.2771675625146002E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.0582005141388099E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.35933629352652E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.6770600607618601E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.0005258237905998E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.3061275999065201E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.6302313624678601E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.9717351122819601E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.8886211731713001E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.5630287450338799E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2.20298434213601E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.87824258004206E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.4954428604814199E-2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.17218976396354E-2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>7.7711614863285802E-3</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>4.7039027810236002E-3</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2.5772376723533501E-3</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.8541715354054599E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-20D2-41BC-A4CC-D3FF8B7297D0}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Lee et al (Strip Theory)</c:v>
+            <c:v>Lee, Kim and Goo (2012) (Strip Theory)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -527,7 +376,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="1"/>
           <c:tx>
             <c:v>Present Study (ANSYS)</c:v>
           </c:tx>
@@ -1582,16 +1431,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>224790</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>156210</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>158115</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>529590</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>156210</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>224790</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1918,8 +1767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B099556-9BBC-4418-9EB3-C6B240910963}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1998,7 +1847,7 @@
         <v>9.6199999999999994E-2</v>
       </c>
       <c r="G3">
-        <f>RADIANS(F3)</f>
+        <f t="shared" ref="G3:G22" si="0">RADIANS(F3)</f>
         <v>1.6790067404185449E-3</v>
       </c>
     </row>
@@ -2022,7 +1871,7 @@
         <v>0.26690000000000003</v>
       </c>
       <c r="G4">
-        <f>RADIANS(F4)</f>
+        <f t="shared" si="0"/>
         <v>4.6582837735728664E-3</v>
       </c>
     </row>
@@ -2046,7 +1895,7 @@
         <v>0.57769999999999999</v>
       </c>
       <c r="G5">
-        <f>RADIANS(F5)</f>
+        <f t="shared" si="0"/>
         <v>1.0082767088771242E-2</v>
       </c>
     </row>
@@ -2070,7 +1919,7 @@
         <v>0.98729999999999996</v>
       </c>
       <c r="G6">
-        <f>RADIANS(F6)</f>
+        <f t="shared" si="0"/>
         <v>1.7231635704940015E-2</v>
       </c>
     </row>
@@ -2094,7 +1943,7 @@
         <v>1.3852</v>
       </c>
       <c r="G7">
-        <f>RADIANS(F7)</f>
+        <f t="shared" si="0"/>
         <v>2.4176300798625452E-2</v>
       </c>
     </row>
@@ -2118,7 +1967,7 @@
         <v>1.6546000000000001</v>
       </c>
       <c r="G8">
-        <f>RADIANS(F8)</f>
+        <f t="shared" si="0"/>
         <v>2.8878217803498179E-2</v>
       </c>
     </row>
@@ -2142,7 +1991,7 @@
         <v>1.4597</v>
       </c>
       <c r="G9">
-        <f>RADIANS(F9)</f>
+        <f t="shared" si="0"/>
         <v>2.5476571091361228E-2</v>
       </c>
     </row>
@@ -2166,7 +2015,7 @@
         <v>0.5958</v>
       </c>
       <c r="G10">
-        <f>RADIANS(F10)</f>
+        <f t="shared" si="0"/>
         <v>1.0398671683382215E-2</v>
       </c>
     </row>
@@ -2190,7 +2039,7 @@
         <v>0.1943</v>
       </c>
       <c r="G11">
-        <f>RADIANS(F11)</f>
+        <f t="shared" si="0"/>
         <v>3.3911747366249822E-3</v>
       </c>
     </row>
@@ -2214,7 +2063,7 @@
         <v>0.14419999999999999</v>
       </c>
       <c r="G12">
-        <f>RADIANS(F12)</f>
+        <f t="shared" si="0"/>
         <v>2.5167647813758233E-3</v>
       </c>
     </row>
@@ -2238,7 +2087,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="G13">
-        <f>RADIANS(F13)</f>
+        <f t="shared" si="0"/>
         <v>7.5049157835756165E-4</v>
       </c>
     </row>
@@ -2262,7 +2111,7 @@
         <v>3.2199999999999999E-2</v>
       </c>
       <c r="G14">
-        <f>RADIANS(F14)</f>
+        <f t="shared" si="0"/>
         <v>5.6199601914217411E-4</v>
       </c>
     </row>
@@ -2286,7 +2135,7 @@
         <v>9.4999999999999998E-3</v>
       </c>
       <c r="G15">
-        <f>RADIANS(F15)</f>
+        <f t="shared" si="0"/>
         <v>1.658062789394613E-4</v>
       </c>
     </row>
@@ -2310,7 +2159,7 @@
         <v>5.1999999999999998E-3</v>
       </c>
       <c r="G16">
-        <f>RADIANS(F16)</f>
+        <f t="shared" si="0"/>
         <v>9.0757121103705133E-5</v>
       </c>
     </row>
@@ -2334,7 +2183,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="G17">
-        <f>RADIANS(F17)</f>
+        <f t="shared" si="0"/>
         <v>4.3633231299858241E-5</v>
       </c>
     </row>
@@ -2358,7 +2207,7 @@
         <v>1.4E-3</v>
       </c>
       <c r="G18">
-        <f>RADIANS(F18)</f>
+        <f t="shared" si="0"/>
         <v>2.4434609527920612E-5</v>
       </c>
     </row>
@@ -2382,7 +2231,7 @@
         <v>4.0000000000000002E-4</v>
       </c>
       <c r="G19">
-        <f>RADIANS(F19)</f>
+        <f t="shared" si="0"/>
         <v>6.9813170079773184E-6</v>
       </c>
     </row>
@@ -2406,7 +2255,7 @@
         <v>0</v>
       </c>
       <c r="G20">
-        <f>RADIANS(F20)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2424,7 +2273,7 @@
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="G21">
-        <f>RADIANS(F21)</f>
+        <f t="shared" si="0"/>
         <v>5.2359877559829886E-6</v>
       </c>
     </row>
@@ -2442,7 +2291,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="G22">
-        <f>RADIANS(F22)</f>
+        <f t="shared" si="0"/>
         <v>3.4906585039886592E-6</v>
       </c>
     </row>

</xml_diff>